<commit_message>
Not sure what I updated, but the binary for this test Excel file is different according to Git, so I guess why not commit!
</commit_message>
<xml_diff>
--- a/data_architect_misc/data_transformer/excel2.xlsx
+++ b/data_architect_misc/data_transformer/excel2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phyo.thiha\Desktop\others\data_architect_misc\data_transformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lache\Documents\GitHub\others\data_architect_misc\data_transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D124167F-1B99-4502-9E0F-2945CB117A2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F9FD5-4A31-46E3-AE20-6EE1F1190945}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{FCEE7782-9213-40EB-9AC9-83CEA33A3CB2}"/>
+    <workbookView xWindow="38760" yWindow="1500" windowWidth="21600" windowHeight="11385" xr2:uid="{FCEE7782-9213-40EB-9AC9-83CEA33A3CB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -637,7 +637,7 @@
   <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated test config files, and the test excel file with a complex scenario to read.
</commit_message>
<xml_diff>
--- a/data_architect_misc/data_transformer/excel2.xlsx
+++ b/data_architect_misc/data_transformer/excel2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lache\Documents\GitHub\others\data_architect_misc\data_transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F9FD5-4A31-46E3-AE20-6EE1F1190945}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7A8F32-C411-45AA-8836-B02E9BA4603E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38760" yWindow="1500" windowWidth="21600" windowHeight="11385" xr2:uid="{FCEE7782-9213-40EB-9AC9-83CEA33A3CB2}"/>
+    <workbookView xWindow="42060" yWindow="-1560" windowWidth="15540" windowHeight="13740" xr2:uid="{FCEE7782-9213-40EB-9AC9-83CEA33A3CB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>Test extra info header line that must be discarded.</t>
   </si>
@@ -230,10 +230,13 @@
     <t>895</t>
   </si>
   <si>
-    <t>Test extra info footer line#1 that must be discarded</t>
-  </si>
-  <si>
-    <t>Test extra info footer line#2 that must be discarded</t>
+    <t>Line#1 to drop</t>
+  </si>
+  <si>
+    <t>Line#2 to drop</t>
+  </si>
+  <si>
+    <t>Line#3 to drop</t>
   </si>
 </sst>
 </file>
@@ -634,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1926ABE5-D524-4E85-AFBD-07C0DBC01CAF}">
-  <dimension ref="A2:E26"/>
+  <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,55 +1009,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>1</v>
+      <c r="B28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>